<commit_message>
aggiungi file comandi github
</commit_message>
<xml_diff>
--- a/RNAscope/Output data analysis/WT_C57BL6_m2-3/classificazione_finale_VIP_positive.xlsx
+++ b/RNAscope/Output data analysis/WT_C57BL6_m2-3/classificazione_finale_VIP_positive.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manuel.felline\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelfelline/Desktop/streamlit-dashboard/RNAscope/Output data analysis/WT_C57BL6_m2-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B063A6-E8EA-374C-9353-B2BAB243B517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classificato" sheetId="1" r:id="rId1"/>
@@ -234,7 +235,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -247,6 +248,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -590,14 +592,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z428"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -677,7 +681,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -757,7 +761,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -837,7 +841,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -917,7 +921,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -997,7 +1001,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1077,7 +1081,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1157,7 +1161,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1237,7 +1241,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1317,7 +1321,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1397,7 +1401,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1477,7 +1481,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1557,7 +1561,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1637,7 +1641,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1717,7 +1721,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1797,7 +1801,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1877,7 +1881,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1957,7 +1961,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -2037,7 +2041,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -2117,7 +2121,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -2197,7 +2201,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2277,7 +2281,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2357,7 +2361,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2437,7 +2441,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2517,7 +2521,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -2597,7 +2601,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -2677,7 +2681,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2757,7 +2761,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2837,7 +2841,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2917,7 +2921,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -2997,7 +3001,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -3077,7 +3081,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -3157,7 +3161,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -3237,7 +3241,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -3317,7 +3321,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
@@ -3397,7 +3401,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
@@ -3477,7 +3481,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -3557,7 +3561,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -3637,7 +3641,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -3717,7 +3721,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
@@ -3797,7 +3801,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
@@ -3877,7 +3881,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
@@ -3957,7 +3961,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1</v>
       </c>
@@ -4037,7 +4041,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1</v>
       </c>
@@ -4117,7 +4121,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1</v>
       </c>
@@ -4197,7 +4201,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1</v>
       </c>
@@ -4277,7 +4281,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1</v>
       </c>
@@ -4357,7 +4361,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1</v>
       </c>
@@ -4437,7 +4441,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1</v>
       </c>
@@ -4517,7 +4521,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1</v>
       </c>
@@ -4597,7 +4601,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1</v>
       </c>
@@ -4677,7 +4681,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1</v>
       </c>
@@ -4757,7 +4761,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1</v>
       </c>
@@ -4837,7 +4841,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1</v>
       </c>
@@ -4917,7 +4921,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1</v>
       </c>
@@ -4997,7 +5001,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1</v>
       </c>
@@ -5077,7 +5081,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1</v>
       </c>
@@ -5157,7 +5161,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1</v>
       </c>
@@ -5237,7 +5241,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1</v>
       </c>
@@ -5317,7 +5321,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1</v>
       </c>
@@ -5397,7 +5401,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1</v>
       </c>
@@ -5477,7 +5481,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1</v>
       </c>
@@ -5557,7 +5561,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1</v>
       </c>
@@ -5637,7 +5641,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1</v>
       </c>
@@ -5717,7 +5721,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>1</v>
       </c>
@@ -5797,7 +5801,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>1</v>
       </c>
@@ -5877,7 +5881,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>1</v>
       </c>
@@ -5957,7 +5961,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>1</v>
       </c>
@@ -6037,7 +6041,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>1</v>
       </c>
@@ -6117,7 +6121,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>1</v>
       </c>
@@ -6197,7 +6201,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>1</v>
       </c>
@@ -6277,7 +6281,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>1</v>
       </c>
@@ -6357,7 +6361,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1</v>
       </c>
@@ -6437,7 +6441,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1</v>
       </c>
@@ -6517,7 +6521,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>1</v>
       </c>
@@ -6597,7 +6601,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>1</v>
       </c>
@@ -6677,7 +6681,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>1</v>
       </c>
@@ -6757,7 +6761,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>1</v>
       </c>
@@ -6837,7 +6841,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>1</v>
       </c>
@@ -6917,7 +6921,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>1</v>
       </c>
@@ -6997,7 +7001,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>1</v>
       </c>
@@ -7077,7 +7081,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1</v>
       </c>
@@ -7157,7 +7161,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>1</v>
       </c>
@@ -7237,7 +7241,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1</v>
       </c>
@@ -7317,7 +7321,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>1</v>
       </c>
@@ -7397,7 +7401,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>1</v>
       </c>
@@ -7477,7 +7481,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1</v>
       </c>
@@ -7557,7 +7561,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>1</v>
       </c>
@@ -7637,7 +7641,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1</v>
       </c>
@@ -7717,7 +7721,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>1</v>
       </c>
@@ -7797,7 +7801,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>1</v>
       </c>
@@ -7877,7 +7881,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>1</v>
       </c>
@@ -7957,7 +7961,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>1</v>
       </c>
@@ -8037,7 +8041,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>1</v>
       </c>
@@ -8117,7 +8121,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>1</v>
       </c>
@@ -8197,7 +8201,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>1</v>
       </c>
@@ -8277,7 +8281,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>1</v>
       </c>
@@ -8357,7 +8361,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>1</v>
       </c>
@@ -8437,7 +8441,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>1</v>
       </c>
@@ -8517,7 +8521,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>1</v>
       </c>
@@ -8597,7 +8601,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>1</v>
       </c>
@@ -8677,7 +8681,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>1</v>
       </c>
@@ -8757,7 +8761,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>1</v>
       </c>
@@ -8837,7 +8841,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>1</v>
       </c>
@@ -8917,7 +8921,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>1</v>
       </c>
@@ -8997,7 +9001,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>1</v>
       </c>
@@ -9077,7 +9081,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>1</v>
       </c>
@@ -9157,7 +9161,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="108" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>1</v>
       </c>
@@ -9237,7 +9241,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="109" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>1</v>
       </c>
@@ -9317,7 +9321,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="110" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>1</v>
       </c>
@@ -9397,7 +9401,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="111" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>1</v>
       </c>
@@ -9477,7 +9481,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="112" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>1</v>
       </c>
@@ -9557,7 +9561,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="113" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>1</v>
       </c>
@@ -9637,7 +9641,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="114" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>1</v>
       </c>
@@ -9717,7 +9721,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="115" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>1</v>
       </c>
@@ -9797,7 +9801,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="116" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>1</v>
       </c>
@@ -9877,7 +9881,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="117" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>1</v>
       </c>
@@ -9957,7 +9961,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="118" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>1</v>
       </c>
@@ -10037,7 +10041,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="119" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>1</v>
       </c>
@@ -10117,7 +10121,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="120" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>1</v>
       </c>
@@ -10197,7 +10201,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="121" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>1</v>
       </c>
@@ -10277,7 +10281,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="122" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>1</v>
       </c>
@@ -10357,7 +10361,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="123" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>1</v>
       </c>
@@ -10437,7 +10441,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="124" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>1</v>
       </c>
@@ -10517,7 +10521,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="125" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>1</v>
       </c>
@@ -10597,7 +10601,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="126" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>1</v>
       </c>
@@ -10677,7 +10681,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="127" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>1</v>
       </c>
@@ -10757,7 +10761,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="128" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>1</v>
       </c>
@@ -10837,7 +10841,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="129" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>1</v>
       </c>
@@ -10917,7 +10921,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="130" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>1</v>
       </c>
@@ -10997,7 +11001,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="131" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>1</v>
       </c>
@@ -11077,7 +11081,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="132" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>1</v>
       </c>
@@ -11157,7 +11161,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="133" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>1</v>
       </c>
@@ -11237,7 +11241,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="134" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>1</v>
       </c>
@@ -11317,7 +11321,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="135" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>1</v>
       </c>
@@ -11397,7 +11401,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="136" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>1</v>
       </c>
@@ -11477,7 +11481,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="137" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>1</v>
       </c>
@@ -11557,7 +11561,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="138" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>1</v>
       </c>
@@ -11637,7 +11641,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="139" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>1</v>
       </c>
@@ -11717,7 +11721,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="140" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>1</v>
       </c>
@@ -11797,7 +11801,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="141" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>1</v>
       </c>
@@ -11877,7 +11881,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="142" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>1</v>
       </c>
@@ -11957,7 +11961,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="143" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>1</v>
       </c>
@@ -12037,7 +12041,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="144" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>1</v>
       </c>
@@ -12117,7 +12121,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="145" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>1</v>
       </c>
@@ -12197,7 +12201,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="146" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>1</v>
       </c>
@@ -12277,7 +12281,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="147" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>1</v>
       </c>
@@ -12357,7 +12361,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="148" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>1</v>
       </c>
@@ -12437,7 +12441,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="149" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>1</v>
       </c>
@@ -12517,7 +12521,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="150" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>1</v>
       </c>
@@ -12597,7 +12601,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="151" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>1</v>
       </c>
@@ -12677,7 +12681,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="152" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>1</v>
       </c>
@@ -12757,7 +12761,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="153" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>1</v>
       </c>
@@ -12837,7 +12841,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="154" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>1</v>
       </c>
@@ -12917,7 +12921,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="155" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>1</v>
       </c>
@@ -12997,7 +13001,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="156" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>1</v>
       </c>
@@ -13077,7 +13081,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="157" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>1</v>
       </c>
@@ -13157,7 +13161,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="158" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>1</v>
       </c>
@@ -13237,7 +13241,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="159" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>1</v>
       </c>
@@ -13317,7 +13321,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="160" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>1</v>
       </c>
@@ -13397,7 +13401,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="161" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>1</v>
       </c>
@@ -13477,7 +13481,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="162" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>1</v>
       </c>
@@ -13557,7 +13561,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="163" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>1</v>
       </c>
@@ -13637,7 +13641,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="164" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>1</v>
       </c>
@@ -13717,7 +13721,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="165" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>1</v>
       </c>
@@ -13797,7 +13801,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="166" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>1</v>
       </c>
@@ -13877,7 +13881,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="167" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>1</v>
       </c>
@@ -13957,7 +13961,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="168" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>1</v>
       </c>
@@ -14037,7 +14041,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="169" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>1</v>
       </c>
@@ -14117,7 +14121,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="170" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>1</v>
       </c>
@@ -14197,7 +14201,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="171" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>1</v>
       </c>
@@ -14277,7 +14281,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="172" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>1</v>
       </c>
@@ -14357,7 +14361,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="173" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>1</v>
       </c>
@@ -14437,7 +14441,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="174" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>1</v>
       </c>
@@ -14517,7 +14521,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="175" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>1</v>
       </c>
@@ -14597,7 +14601,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="176" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>1</v>
       </c>
@@ -14677,7 +14681,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="177" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>1</v>
       </c>
@@ -14757,7 +14761,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="178" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>1</v>
       </c>
@@ -14837,7 +14841,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="179" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>1</v>
       </c>
@@ -14917,7 +14921,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="180" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>1</v>
       </c>
@@ -14997,7 +15001,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="181" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>1</v>
       </c>
@@ -15077,7 +15081,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="182" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>1</v>
       </c>
@@ -15157,7 +15161,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="183" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>1</v>
       </c>
@@ -15237,7 +15241,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="184" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>1</v>
       </c>
@@ -15317,7 +15321,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="185" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>1</v>
       </c>
@@ -15397,7 +15401,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="186" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>1</v>
       </c>
@@ -15477,7 +15481,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="187" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>1</v>
       </c>
@@ -15557,7 +15561,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="188" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>1</v>
       </c>
@@ -15637,7 +15641,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="189" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>1</v>
       </c>
@@ -15717,7 +15721,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="190" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>1</v>
       </c>
@@ -15797,7 +15801,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="191" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>1</v>
       </c>
@@ -15877,7 +15881,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="192" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>1</v>
       </c>
@@ -15957,7 +15961,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="193" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>1</v>
       </c>
@@ -16037,7 +16041,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="194" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>1</v>
       </c>
@@ -16117,7 +16121,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="195" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>1</v>
       </c>
@@ -16197,7 +16201,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="196" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>1</v>
       </c>
@@ -16277,7 +16281,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="197" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>1</v>
       </c>
@@ -16357,7 +16361,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="198" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>1</v>
       </c>
@@ -16437,7 +16441,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="199" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>1</v>
       </c>
@@ -16517,7 +16521,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="200" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>1</v>
       </c>
@@ -16597,7 +16601,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="201" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>1</v>
       </c>
@@ -16677,7 +16681,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="202" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>1</v>
       </c>
@@ -16757,7 +16761,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="203" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>1</v>
       </c>
@@ -16837,7 +16841,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="204" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>1</v>
       </c>
@@ -16917,7 +16921,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="205" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>1</v>
       </c>
@@ -16997,7 +17001,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="206" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>1</v>
       </c>
@@ -17077,7 +17081,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="207" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>1</v>
       </c>
@@ -17157,7 +17161,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="208" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>1</v>
       </c>
@@ -17237,7 +17241,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="209" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>1</v>
       </c>
@@ -17317,7 +17321,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="210" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>1</v>
       </c>
@@ -17397,7 +17401,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="211" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>1</v>
       </c>
@@ -17477,7 +17481,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="212" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>1</v>
       </c>
@@ -17557,7 +17561,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="213" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>1</v>
       </c>
@@ -17637,7 +17641,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="214" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>1</v>
       </c>
@@ -17717,7 +17721,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="215" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>1</v>
       </c>
@@ -17797,7 +17801,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="216" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>1</v>
       </c>
@@ -17877,7 +17881,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="217" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>1</v>
       </c>
@@ -17957,7 +17961,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="218" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>1</v>
       </c>
@@ -18037,7 +18041,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="219" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>1</v>
       </c>
@@ -18117,7 +18121,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="220" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>1</v>
       </c>
@@ -18197,7 +18201,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="221" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>1</v>
       </c>
@@ -18277,7 +18281,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="222" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>1</v>
       </c>
@@ -18357,7 +18361,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="223" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>1</v>
       </c>
@@ -18437,7 +18441,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="224" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>1</v>
       </c>
@@ -18517,7 +18521,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="225" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>1</v>
       </c>
@@ -18597,7 +18601,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="226" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>1</v>
       </c>
@@ -18677,7 +18681,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="227" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>1</v>
       </c>
@@ -18757,7 +18761,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="228" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>1</v>
       </c>
@@ -18837,7 +18841,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="229" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>1</v>
       </c>
@@ -18917,7 +18921,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="230" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>1</v>
       </c>
@@ -18997,7 +19001,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="231" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>1</v>
       </c>
@@ -19077,7 +19081,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="232" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>1</v>
       </c>
@@ -19157,7 +19161,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="233" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>1</v>
       </c>
@@ -19237,7 +19241,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="234" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>1</v>
       </c>
@@ -19317,7 +19321,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="235" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>1</v>
       </c>
@@ -19397,7 +19401,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="236" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>1</v>
       </c>
@@ -19477,7 +19481,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="237" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>1</v>
       </c>
@@ -19557,7 +19561,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="238" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>1</v>
       </c>
@@ -19637,7 +19641,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="239" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>1</v>
       </c>
@@ -19717,7 +19721,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="240" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>1</v>
       </c>
@@ -19797,7 +19801,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="241" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>1</v>
       </c>
@@ -19877,7 +19881,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="242" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>1</v>
       </c>
@@ -19957,7 +19961,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="243" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>1</v>
       </c>
@@ -20037,7 +20041,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="244" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>1</v>
       </c>
@@ -20117,7 +20121,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="245" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>1</v>
       </c>
@@ -20197,7 +20201,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="246" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>1</v>
       </c>
@@ -20277,7 +20281,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="247" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>1</v>
       </c>
@@ -20357,7 +20361,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="248" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>1</v>
       </c>
@@ -20437,7 +20441,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="249" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>1</v>
       </c>
@@ -20517,7 +20521,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="250" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>1</v>
       </c>
@@ -20597,7 +20601,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="251" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>1</v>
       </c>
@@ -20677,7 +20681,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="252" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>1</v>
       </c>
@@ -20757,7 +20761,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="253" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>1</v>
       </c>
@@ -20837,7 +20841,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="254" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>1</v>
       </c>
@@ -20917,7 +20921,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="255" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>1</v>
       </c>
@@ -20997,7 +21001,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="256" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>1</v>
       </c>
@@ -21077,7 +21081,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="257" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>1</v>
       </c>
@@ -21157,7 +21161,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="258" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>1</v>
       </c>
@@ -21237,7 +21241,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="259" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>1</v>
       </c>
@@ -21317,7 +21321,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="260" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>1</v>
       </c>
@@ -21397,7 +21401,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="261" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>1</v>
       </c>
@@ -21477,7 +21481,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="262" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>1</v>
       </c>
@@ -21557,7 +21561,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="263" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>1</v>
       </c>
@@ -21637,7 +21641,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="264" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>1</v>
       </c>
@@ -21717,7 +21721,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="265" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>1</v>
       </c>
@@ -21797,7 +21801,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="266" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>1</v>
       </c>
@@ -21877,7 +21881,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="267" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>1</v>
       </c>
@@ -21957,7 +21961,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="268" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>1</v>
       </c>
@@ -22037,7 +22041,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="269" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>1</v>
       </c>
@@ -22117,7 +22121,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="270" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>1</v>
       </c>
@@ -22197,7 +22201,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="271" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>1</v>
       </c>
@@ -22277,7 +22281,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="272" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>1</v>
       </c>
@@ -22357,7 +22361,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="273" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>1</v>
       </c>
@@ -22437,7 +22441,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="274" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>1</v>
       </c>
@@ -22517,7 +22521,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="275" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>1</v>
       </c>
@@ -22597,7 +22601,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="276" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>1</v>
       </c>
@@ -22677,7 +22681,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="277" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>1</v>
       </c>
@@ -22757,7 +22761,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="278" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>1</v>
       </c>
@@ -22837,7 +22841,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="279" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>1</v>
       </c>
@@ -22917,7 +22921,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="280" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>1</v>
       </c>
@@ -22997,7 +23001,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="281" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>1</v>
       </c>
@@ -23077,7 +23081,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="282" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>1</v>
       </c>
@@ -23157,7 +23161,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="283" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>1</v>
       </c>
@@ -23237,7 +23241,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="284" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>1</v>
       </c>
@@ -23317,7 +23321,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="285" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>1</v>
       </c>
@@ -23397,7 +23401,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="286" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>1</v>
       </c>
@@ -23477,7 +23481,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="287" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>1</v>
       </c>
@@ -23557,7 +23561,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="288" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>1</v>
       </c>
@@ -23637,7 +23641,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="289" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>1</v>
       </c>
@@ -23717,7 +23721,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="290" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>1</v>
       </c>
@@ -23797,7 +23801,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="291" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>1</v>
       </c>
@@ -23877,7 +23881,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="292" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>1</v>
       </c>
@@ -23957,7 +23961,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="293" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>1</v>
       </c>
@@ -24037,7 +24041,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="294" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>1</v>
       </c>
@@ -24117,7 +24121,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="295" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>1</v>
       </c>
@@ -24197,7 +24201,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="296" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>1</v>
       </c>
@@ -24277,7 +24281,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="297" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>1</v>
       </c>
@@ -24357,7 +24361,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="298" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>1</v>
       </c>
@@ -24437,7 +24441,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="299" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>1</v>
       </c>
@@ -24517,7 +24521,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="300" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>1</v>
       </c>
@@ -24597,7 +24601,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="301" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>1</v>
       </c>
@@ -24677,7 +24681,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="302" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>1</v>
       </c>
@@ -24757,7 +24761,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="303" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>1</v>
       </c>
@@ -24837,7 +24841,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="304" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>1</v>
       </c>
@@ -24917,7 +24921,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="305" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>1</v>
       </c>
@@ -24997,7 +25001,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="306" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>1</v>
       </c>
@@ -25077,7 +25081,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="307" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>1</v>
       </c>
@@ -25157,7 +25161,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="308" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>1</v>
       </c>
@@ -25237,7 +25241,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="309" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>1</v>
       </c>
@@ -25317,7 +25321,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="310" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>1</v>
       </c>
@@ -25397,7 +25401,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="311" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>1</v>
       </c>
@@ -25477,7 +25481,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="312" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>1</v>
       </c>
@@ -25557,7 +25561,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="313" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>1</v>
       </c>
@@ -25637,7 +25641,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="314" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>1</v>
       </c>
@@ -25717,7 +25721,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="315" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>1</v>
       </c>
@@ -25797,7 +25801,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="316" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>1</v>
       </c>
@@ -25877,7 +25881,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="317" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A317">
         <v>1</v>
       </c>
@@ -25957,7 +25961,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="318" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A318">
         <v>1</v>
       </c>
@@ -26037,7 +26041,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="319" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>1</v>
       </c>
@@ -26117,7 +26121,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="320" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A320">
         <v>1</v>
       </c>
@@ -26197,7 +26201,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="321" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>1</v>
       </c>
@@ -26277,7 +26281,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="322" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>1</v>
       </c>
@@ -26357,7 +26361,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="323" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>1</v>
       </c>
@@ -26437,7 +26441,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="324" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A324">
         <v>1</v>
       </c>
@@ -26517,7 +26521,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="325" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>1</v>
       </c>
@@ -26597,7 +26601,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="326" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A326">
         <v>1</v>
       </c>
@@ -26677,7 +26681,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="327" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>1</v>
       </c>
@@ -26757,7 +26761,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="328" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>1</v>
       </c>
@@ -26837,7 +26841,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="329" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>1</v>
       </c>
@@ -26917,7 +26921,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="330" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>1</v>
       </c>
@@ -26997,7 +27001,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="331" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>1</v>
       </c>
@@ -27077,7 +27081,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="332" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>1</v>
       </c>
@@ -27157,7 +27161,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="333" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A333">
         <v>1</v>
       </c>
@@ -27237,7 +27241,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="334" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A334">
         <v>1</v>
       </c>
@@ -27317,7 +27321,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="335" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A335">
         <v>1</v>
       </c>
@@ -27397,7 +27401,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="336" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A336">
         <v>1</v>
       </c>
@@ -27477,7 +27481,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="337" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>1</v>
       </c>
@@ -27557,7 +27561,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="338" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A338">
         <v>1</v>
       </c>
@@ -27637,7 +27641,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="339" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A339">
         <v>1</v>
       </c>
@@ -27717,7 +27721,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="340" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>1</v>
       </c>
@@ -27797,7 +27801,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="341" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A341">
         <v>1</v>
       </c>
@@ -27877,7 +27881,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="342" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A342">
         <v>1</v>
       </c>
@@ -27957,7 +27961,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="343" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A343">
         <v>1</v>
       </c>
@@ -28037,7 +28041,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="344" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A344">
         <v>1</v>
       </c>
@@ -28117,7 +28121,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="345" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A345">
         <v>1</v>
       </c>
@@ -28197,7 +28201,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="346" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A346">
         <v>1</v>
       </c>
@@ -28277,7 +28281,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="347" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A347">
         <v>1</v>
       </c>
@@ -28357,7 +28361,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="348" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A348">
         <v>1</v>
       </c>
@@ -28437,7 +28441,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="349" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A349">
         <v>1</v>
       </c>
@@ -28517,7 +28521,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="350" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A350">
         <v>1</v>
       </c>
@@ -28597,7 +28601,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="351" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A351">
         <v>1</v>
       </c>
@@ -28677,7 +28681,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="352" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A352">
         <v>1</v>
       </c>
@@ -28757,7 +28761,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="353" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A353">
         <v>1</v>
       </c>
@@ -28837,7 +28841,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="354" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A354">
         <v>1</v>
       </c>
@@ -28917,7 +28921,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="355" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A355">
         <v>1</v>
       </c>
@@ -28997,7 +29001,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="356" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A356">
         <v>1</v>
       </c>
@@ -29077,7 +29081,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="357" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A357">
         <v>1</v>
       </c>
@@ -29157,7 +29161,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="358" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A358">
         <v>1</v>
       </c>
@@ -29237,7 +29241,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="359" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A359">
         <v>1</v>
       </c>
@@ -29317,7 +29321,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="360" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A360">
         <v>1</v>
       </c>
@@ -29397,7 +29401,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="361" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A361">
         <v>1</v>
       </c>
@@ -29477,7 +29481,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="362" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A362">
         <v>1</v>
       </c>
@@ -29557,7 +29561,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="363" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A363">
         <v>1</v>
       </c>
@@ -29637,7 +29641,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="364" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A364">
         <v>1</v>
       </c>
@@ -29717,7 +29721,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="365" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A365">
         <v>1</v>
       </c>
@@ -29797,7 +29801,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="366" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A366">
         <v>1</v>
       </c>
@@ -29877,7 +29881,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="367" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A367">
         <v>1</v>
       </c>
@@ -29957,7 +29961,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="368" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A368">
         <v>1</v>
       </c>
@@ -30037,7 +30041,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="369" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A369">
         <v>1</v>
       </c>
@@ -30117,7 +30121,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="370" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A370">
         <v>1</v>
       </c>
@@ -30197,7 +30201,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="371" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A371">
         <v>1</v>
       </c>
@@ -30277,7 +30281,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="372" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A372">
         <v>1</v>
       </c>
@@ -30357,7 +30361,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="373" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A373">
         <v>1</v>
       </c>
@@ -30437,7 +30441,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="374" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A374">
         <v>1</v>
       </c>
@@ -30517,7 +30521,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="375" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A375">
         <v>1</v>
       </c>
@@ -30597,7 +30601,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="376" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A376">
         <v>1</v>
       </c>
@@ -30677,7 +30681,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="377" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A377">
         <v>1</v>
       </c>
@@ -30757,7 +30761,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="378" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A378">
         <v>1</v>
       </c>
@@ -30837,7 +30841,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="379" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A379">
         <v>1</v>
       </c>
@@ -30917,7 +30921,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="380" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A380">
         <v>1</v>
       </c>
@@ -30997,7 +31001,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="381" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A381">
         <v>1</v>
       </c>
@@ -31077,7 +31081,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="382" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A382">
         <v>1</v>
       </c>
@@ -31157,7 +31161,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="383" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A383">
         <v>1</v>
       </c>
@@ -31237,7 +31241,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="384" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A384">
         <v>1</v>
       </c>
@@ -31317,7 +31321,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="385" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A385">
         <v>1</v>
       </c>
@@ -31397,7 +31401,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="386" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A386">
         <v>1</v>
       </c>
@@ -31477,7 +31481,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="387" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A387">
         <v>1</v>
       </c>
@@ -31557,7 +31561,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="388" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A388">
         <v>1</v>
       </c>
@@ -31637,7 +31641,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="389" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A389">
         <v>1</v>
       </c>
@@ -31717,7 +31721,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="390" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A390">
         <v>1</v>
       </c>
@@ -31797,7 +31801,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="391" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A391">
         <v>1</v>
       </c>
@@ -31877,7 +31881,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="392" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A392">
         <v>1</v>
       </c>
@@ -31957,7 +31961,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="393" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A393">
         <v>1</v>
       </c>
@@ -32037,7 +32041,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="394" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A394">
         <v>1</v>
       </c>
@@ -32117,7 +32121,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="395" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A395">
         <v>1</v>
       </c>
@@ -32197,7 +32201,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="396" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A396">
         <v>1</v>
       </c>
@@ -32277,7 +32281,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="397" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A397">
         <v>1</v>
       </c>
@@ -32357,7 +32361,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="398" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A398">
         <v>1</v>
       </c>
@@ -32437,7 +32441,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="399" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A399">
         <v>1</v>
       </c>
@@ -32517,7 +32521,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="400" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A400">
         <v>1</v>
       </c>
@@ -32597,7 +32601,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="401" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A401">
         <v>1</v>
       </c>
@@ -32677,7 +32681,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="402" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A402">
         <v>1</v>
       </c>
@@ -32757,7 +32761,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="403" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A403">
         <v>1</v>
       </c>
@@ -32837,7 +32841,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="404" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A404">
         <v>1</v>
       </c>
@@ -32917,7 +32921,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="405" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A405">
         <v>1</v>
       </c>
@@ -32997,7 +33001,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="406" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A406">
         <v>1</v>
       </c>
@@ -33077,7 +33081,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="407" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A407">
         <v>1</v>
       </c>
@@ -33157,7 +33161,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="408" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A408">
         <v>1</v>
       </c>
@@ -33237,7 +33241,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="409" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A409">
         <v>1</v>
       </c>
@@ -33317,7 +33321,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="410" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A410">
         <v>1</v>
       </c>
@@ -33397,7 +33401,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="411" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A411">
         <v>1</v>
       </c>
@@ -33477,7 +33481,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="412" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A412">
         <v>1</v>
       </c>
@@ -33557,7 +33561,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="413" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A413">
         <v>1</v>
       </c>
@@ -33637,7 +33641,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="414" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A414">
         <v>1</v>
       </c>
@@ -33717,7 +33721,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="415" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A415">
         <v>1</v>
       </c>
@@ -33797,7 +33801,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="416" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A416">
         <v>1</v>
       </c>
@@ -33877,7 +33881,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="417" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A417">
         <v>1</v>
       </c>
@@ -33957,7 +33961,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="418" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A418">
         <v>1</v>
       </c>
@@ -34037,7 +34041,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="419" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A419">
         <v>1</v>
       </c>
@@ -34117,7 +34121,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="420" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A420">
         <v>1</v>
       </c>
@@ -34197,7 +34201,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="421" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A421">
         <v>1</v>
       </c>
@@ -34277,7 +34281,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="422" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A422">
         <v>1</v>
       </c>
@@ -34357,7 +34361,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="423" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A423">
         <v>1</v>
       </c>
@@ -34437,7 +34441,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="424" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A424">
         <v>1</v>
       </c>
@@ -34517,7 +34521,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="425" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A425">
         <v>1</v>
       </c>
@@ -34597,7 +34601,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="426" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A426">
         <v>1</v>
       </c>
@@ -34677,7 +34681,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="427" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A427">
         <v>1</v>
       </c>
@@ -34757,7 +34761,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="428" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A428">
         <v>1</v>
       </c>
@@ -34843,24 +34847,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="29.5" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -34883,7 +34887,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -34906,7 +34910,7 @@
         <v>4.0983606557377046</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -34929,7 +34933,7 @@
         <v>3.8461538461538458</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -34958,14 +34962,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -34988,7 +34992,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -35011,7 +35015,7 @@
         <v>11.47540983606557</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -35034,7 +35038,7 @@
         <v>2.884615384615385</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -35063,14 +35067,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -35078,7 +35082,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -35086,7 +35090,7 @@
         <v>23.770491803278691</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -35094,7 +35098,7 @@
         <v>15.38461538461539</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -35108,14 +35112,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -35123,7 +35130,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -35131,7 +35138,7 @@
         <v>36.065573770491802</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -35139,7 +35146,7 @@
         <v>26.92307692307692</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -35153,14 +35160,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -35168,7 +35175,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -35176,7 +35183,7 @@
         <v>12.295081967213109</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -35184,7 +35191,7 @@
         <v>7.6923076923076934</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -35198,14 +35205,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="20" width="36" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -35264,7 +35276,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -35323,7 +35335,7 @@
         <v>0.81967213114754101</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -35364,7 +35376,7 @@
         <v>3.8461538461538458</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>40</v>
       </c>

</xml_diff>